<commit_message>
Deleted Pivot Table Column, Change to Product, Modify Cell
</commit_message>
<xml_diff>
--- a/pivot-table.xlsx
+++ b/pivot-table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shubhamkumar/Downloads/xlsx-experiments/dogshit/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shubhamkumar/Documents/git-repos/xlsx-vcs-experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9CEFF58-6E01-A34D-8943-A25E39FF2106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A33C085-C2A8-BC40-947F-BC8E2BC795B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="20420" activeTab="1" xr2:uid="{A77D4A2C-567D-4C9D-8921-4BDC69E3756D}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="97">
   <si>
     <t>Income Statement:</t>
   </si>
@@ -322,12 +322,6 @@
     <t>Sum of servers</t>
   </si>
   <si>
-    <t>Sum of 1 qps</t>
-  </si>
-  <si>
-    <t>Min of 100 qps</t>
-  </si>
-  <si>
     <t>Sum of 1000 qps</t>
   </si>
   <si>
@@ -335,6 +329,9 @@
   </si>
   <si>
     <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Product of 1 qps</t>
   </si>
 </sst>
 </file>
@@ -446,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -491,6 +488,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,12 +627,12 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1D1FEEEC-3AD1-C94D-84F4-AE39F46C8822}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:E14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1D1FEEEC-3AD1-C94D-84F4-AE39F46C8822}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:D14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField axis="axisRow" dataField="1" showAll="0">
       <items count="11">
         <item x="1"/>
@@ -692,7 +690,7 @@
   <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="4">
+  <colItems count="3">
     <i>
       <x/>
     </i>
@@ -702,14 +700,10 @@
     <i i="2">
       <x v="2"/>
     </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
   </colItems>
-  <dataFields count="4">
+  <dataFields count="3">
     <dataField name="Sum of 1000 qps" fld="3" baseField="0" baseItem="0"/>
-    <dataField name="Min of 100 qps" fld="2" subtotal="min" baseField="0" baseItem="0"/>
-    <dataField name="Sum of 1 qps" fld="1" baseField="0" baseItem="0"/>
+    <dataField name="Product of 1 qps" fld="1" subtotal="product" baseField="0" baseItem="0"/>
     <dataField name="Sum of servers" fld="0" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -4027,222 +4021,185 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC037E77-15B1-CF44-9FF4-CA2D8BDFCC84}">
-  <dimension ref="A3:E20"/>
+  <dimension ref="A3:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" t="s">
         <v>96</v>
       </c>
-      <c r="B3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" t="s">
-        <v>94</v>
-      </c>
       <c r="D3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="33">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="34">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>45</v>
-      </c>
-      <c r="D4">
+      <c r="C4" s="34">
         <v>14</v>
       </c>
-      <c r="E4">
+      <c r="D4" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="33">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="34">
         <v>3</v>
       </c>
-      <c r="C5">
-        <v>268</v>
-      </c>
-      <c r="D5">
+      <c r="C5" s="34">
         <v>3</v>
       </c>
-      <c r="E5">
+      <c r="D5" s="34">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="33">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="34">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>46</v>
-      </c>
-      <c r="D6">
+      <c r="C6" s="34">
         <v>432</v>
       </c>
-      <c r="E6">
+      <c r="D6" s="34">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="33">
         <v>23</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="34">
         <v>23</v>
       </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
+      <c r="C7" s="34">
         <v>3</v>
       </c>
-      <c r="E7">
+      <c r="D7" s="34">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="33">
         <v>24</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="34">
         <v>24</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
+      <c r="C8" s="34">
         <v>234</v>
       </c>
-      <c r="E8">
+      <c r="D8" s="34">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="33">
         <v>26</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="34">
         <v>26</v>
       </c>
-      <c r="C9">
-        <v>9</v>
-      </c>
-      <c r="D9">
+      <c r="C9" s="34">
         <v>3</v>
       </c>
-      <c r="E9">
+      <c r="D9" s="34">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="33">
         <v>32</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="34">
         <v>64</v>
       </c>
-      <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <v>7</v>
-      </c>
-      <c r="E10">
+      <c r="C10" s="34">
+        <v>10</v>
+      </c>
+      <c r="D10" s="34">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="33">
         <v>35</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="34">
         <v>35</v>
       </c>
-      <c r="C11">
-        <v>4657</v>
-      </c>
-      <c r="D11">
+      <c r="C11" s="34">
         <v>754</v>
       </c>
-      <c r="E11">
+      <c r="D11" s="34">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="33">
         <v>43</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="34">
         <v>86</v>
       </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12">
-        <v>27</v>
-      </c>
-      <c r="E12">
+      <c r="C12" s="34">
+        <v>180</v>
+      </c>
+      <c r="D12" s="34">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="33">
         <v>2453</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="34">
         <v>2453</v>
       </c>
-      <c r="C13">
-        <v>425</v>
-      </c>
-      <c r="D13">
+      <c r="C13" s="34">
         <v>13</v>
       </c>
-      <c r="E13">
+      <c r="D13" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="B14">
+        <v>95</v>
+      </c>
+      <c r="B14" s="34">
         <v>2721</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>1490</v>
-      </c>
-      <c r="E14">
+      <c r="C14" s="34">
+        <v>674184257510400</v>
+      </c>
+      <c r="D14" s="34">
         <v>24</v>
       </c>
     </row>
@@ -4251,7 +4208,7 @@
         <v>4</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -4278,7 +4235,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D13"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>